<commit_message>
display cards and buttons
</commit_message>
<xml_diff>
--- a/scoringTable.xlsx
+++ b/scoringTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regina\Desktop\Learning\Rocket_Academy\Rocket_Academy_Projects\bootcamp\project5_major_poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42D4E365-1FCA-4A1F-98C3-E43BDDA19C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4899D8-254E-4476-9848-45F0B332B914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="-14220" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
+    <workbookView xWindow="3165" yWindow="3885" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,7 +447,7 @@
   <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,6 +494,9 @@
         <f>_xlfn.FLOOR.MATH(E2)</f>
         <v>649350</v>
       </c>
+      <c r="G2">
+        <v>250</v>
+      </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -514,6 +517,9 @@
         <f t="shared" ref="F3:F11" si="2">_xlfn.FLOOR.MATH(E3)</f>
         <v>71942</v>
       </c>
+      <c r="G3">
+        <v>150</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -534,6 +540,9 @@
         <f t="shared" si="2"/>
         <v>4164</v>
       </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -554,6 +563,9 @@
         <f t="shared" si="2"/>
         <v>693</v>
       </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -574,6 +586,9 @@
         <f t="shared" si="2"/>
         <v>508</v>
       </c>
+      <c r="G6">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -594,6 +609,9 @@
         <f t="shared" si="2"/>
         <v>254</v>
       </c>
+      <c r="G7">
+        <v>45</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -614,6 +632,9 @@
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
+      <c r="G8">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -634,6 +655,9 @@
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
+      <c r="G9">
+        <v>25</v>
+      </c>
       <c r="K9">
         <f>1/0.5</f>
         <v>2</v>
@@ -658,6 +682,9 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
       <c r="K10">
         <f>1/0.0762</f>
         <v>13.123359580052492</v>
@@ -680,6 +707,9 @@
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
winnings for other levels
</commit_message>
<xml_diff>
--- a/scoringTable.xlsx
+++ b/scoringTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regina\Desktop\Learning\Rocket_Academy\Rocket_Academy_Projects\bootcamp\project5_major_poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4899D8-254E-4476-9848-45F0B332B914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22D9B10-6E97-45ED-AC1E-2BD5C9D0AD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="3885" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
+    <workbookView xWindow="5535" yWindow="-13800" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>royal flush</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Rounding</t>
+  </si>
+  <si>
+    <t>loss</t>
   </si>
 </sst>
 </file>
@@ -444,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0881E39-8CD5-40E5-9D02-EF12D2BEF2A9}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,6 +500,14 @@
       <c r="G2">
         <v>250</v>
       </c>
+      <c r="H2">
+        <f>G2*1.5</f>
+        <v>375</v>
+      </c>
+      <c r="I2">
+        <f>G2*2</f>
+        <v>500</v>
+      </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -520,6 +531,14 @@
       <c r="G3">
         <v>150</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H12" si="3">G3*1.5</f>
+        <v>225</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I12" si="4">G3*2</f>
+        <v>300</v>
+      </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -543,6 +562,14 @@
       <c r="G4">
         <v>100</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -566,6 +593,14 @@
       <c r="G5">
         <v>80</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -589,6 +624,14 @@
       <c r="G6">
         <v>60</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -612,6 +655,13 @@
       <c r="G7">
         <v>45</v>
       </c>
+      <c r="H7">
+        <v>68</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -635,6 +685,14 @@
       <c r="G8">
         <v>32</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -658,6 +716,13 @@
       <c r="G9">
         <v>25</v>
       </c>
+      <c r="H9">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
       <c r="K9">
         <f>1/0.5</f>
         <v>2</v>
@@ -685,6 +750,14 @@
       <c r="G10">
         <v>10</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
       <c r="K10">
         <f>1/0.0762</f>
         <v>13.123359580052492</v>
@@ -711,6 +784,29 @@
       </c>
       <c r="G11">
         <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add submit logic n update evaluate wins logic
</commit_message>
<xml_diff>
--- a/scoringTable.xlsx
+++ b/scoringTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regina\Desktop\Learning\Rocket_Academy\Rocket_Academy_Projects\bootcamp\project5_major_poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22D9B10-6E97-45ED-AC1E-2BD5C9D0AD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6513269-EE27-463A-A312-CAE471A14BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="-13800" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
+    <workbookView xWindow="4080" yWindow="5070" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>royal flush</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t>loss</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Power Up</t>
+  </si>
+  <si>
+    <t>Double</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +486,15 @@
       <c r="F1" t="s">
         <v>14</v>
       </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -532,7 +550,7 @@
         <v>150</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H12" si="3">G3*1.5</f>
+        <f t="shared" ref="H3:H11" si="3">G3*1.5</f>
         <v>225</v>
       </c>
       <c r="I3">
@@ -799,14 +817,14 @@
         <v>15</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="H12">
-        <v>8</v>
+        <v>-8</v>
       </c>
       <c r="I12">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exports and bets amounts
</commit_message>
<xml_diff>
--- a/scoringTable.xlsx
+++ b/scoringTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regina\Desktop\Learning\Rocket_Academy\Rocket_Academy_Projects\bootcamp\project5_major_poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6513269-EE27-463A-A312-CAE471A14BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E42B864-35C8-4946-A1FA-18CE597B1060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="5070" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
+    <workbookView xWindow="4080" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,7 +100,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +111,14 @@
     <font>
       <b/>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -138,10 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +469,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,32 +792,32 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="4">
         <v>50.117699999999999</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>1.9953030566047525E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <f t="shared" si="1"/>
         <v>1.9953030566047525</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
@@ -820,11 +830,11 @@
         <v>-5</v>
       </c>
       <c r="H12">
-        <v>-8</v>
+        <v>-10</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
-        <v>-10</v>
+        <f>-20</f>
+        <v>-20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lose and buttons for bets
</commit_message>
<xml_diff>
--- a/scoringTable.xlsx
+++ b/scoringTable.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\regina\Desktop\Learning\Rocket_Academy\Rocket_Academy_Projects\bootcamp\project5_major_poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E42B864-35C8-4946-A1FA-18CE597B1060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B5BFA7-94A2-4C48-89A7-C0BB4C724A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
+    <workbookView xWindow="3300" yWindow="3450" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{54AB92D9-BA7E-433F-B10B-9F9C0C41ECDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>royal flush</t>
   </si>
@@ -91,6 +92,42 @@
   </si>
   <si>
     <t>Double</t>
+  </si>
+  <si>
+    <t>Straight Flush</t>
+  </si>
+  <si>
+    <t>Four of a Kind</t>
+  </si>
+  <si>
+    <t>Full House</t>
+  </si>
+  <si>
+    <t>Flush</t>
+  </si>
+  <si>
+    <t>Straight</t>
+  </si>
+  <si>
+    <t>Three of a Kind</t>
+  </si>
+  <si>
+    <t>Two Pair</t>
+  </si>
+  <si>
+    <t>One Pair</t>
+  </si>
+  <si>
+    <t>Royal Flush</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Lose</t>
+  </si>
+  <si>
+    <t>BETS</t>
   </si>
 </sst>
 </file>
@@ -100,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +162,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAA520"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,18 +217,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDAA520"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -466,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0881E39-8CD5-40E5-9D02-EF12D2BEF2A9}">
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +572,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
@@ -506,7 +598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -536,8 +628,20 @@
         <f>G2*2</f>
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="6">
+        <v>250</v>
+      </c>
+      <c r="O2" s="6">
+        <v>375</v>
+      </c>
+      <c r="P2" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -564,11 +668,23 @@
         <v>225</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I12" si="4">G3*2</f>
+        <f t="shared" ref="I3:I11" si="4">G3*2</f>
         <v>300</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="6">
+        <v>150</v>
+      </c>
+      <c r="O3" s="6">
+        <v>225</v>
+      </c>
+      <c r="P3" s="6">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -598,8 +714,20 @@
         <f t="shared" si="4"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="6">
+        <v>100</v>
+      </c>
+      <c r="O4" s="6">
+        <v>150</v>
+      </c>
+      <c r="P4" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -629,8 +757,20 @@
         <f t="shared" si="4"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="6">
+        <v>80</v>
+      </c>
+      <c r="O5" s="6">
+        <v>120</v>
+      </c>
+      <c r="P5" s="6">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -660,8 +800,20 @@
         <f t="shared" si="4"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="6">
+        <v>60</v>
+      </c>
+      <c r="O6" s="6">
+        <v>90</v>
+      </c>
+      <c r="P6" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -690,8 +842,20 @@
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="6">
+        <v>45</v>
+      </c>
+      <c r="O7" s="6">
+        <v>68</v>
+      </c>
+      <c r="P7" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -721,8 +885,20 @@
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="6">
+        <v>32</v>
+      </c>
+      <c r="O8" s="6">
+        <v>48</v>
+      </c>
+      <c r="P8" s="6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -755,8 +931,20 @@
         <f>1/0.5</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="6">
+        <v>25</v>
+      </c>
+      <c r="O9" s="6">
+        <v>38</v>
+      </c>
+      <c r="P9" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -790,8 +978,20 @@
         <f>1/0.0762</f>
         <v>13.123359580052492</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="M10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="6">
+        <v>10</v>
+      </c>
+      <c r="O10" s="6">
+        <v>15</v>
+      </c>
+      <c r="P10" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -822,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -841,4 +1041,216 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E5B5B7-0910-4451-B718-153CA453A43E}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="17" customWidth="1"/>
+    <col min="3" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="10">
+        <v>250</v>
+      </c>
+      <c r="D3" s="10">
+        <v>375</v>
+      </c>
+      <c r="E3" s="10">
+        <v>500</v>
+      </c>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10">
+        <v>150</v>
+      </c>
+      <c r="D4" s="10">
+        <v>225</v>
+      </c>
+      <c r="E4" s="10">
+        <v>300</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>100</v>
+      </c>
+      <c r="D5" s="10">
+        <v>150</v>
+      </c>
+      <c r="E5" s="10">
+        <v>200</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10">
+        <v>80</v>
+      </c>
+      <c r="D6" s="10">
+        <v>120</v>
+      </c>
+      <c r="E6" s="10">
+        <v>160</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="10">
+        <v>60</v>
+      </c>
+      <c r="D7" s="10">
+        <v>90</v>
+      </c>
+      <c r="E7" s="10">
+        <v>120</v>
+      </c>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="10">
+        <v>45</v>
+      </c>
+      <c r="D8" s="10">
+        <v>68</v>
+      </c>
+      <c r="E8" s="10">
+        <v>90</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="10">
+        <v>32</v>
+      </c>
+      <c r="D9" s="10">
+        <v>48</v>
+      </c>
+      <c r="E9" s="10">
+        <v>64</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="10">
+        <v>25</v>
+      </c>
+      <c r="D10" s="10">
+        <v>38</v>
+      </c>
+      <c r="E10" s="10">
+        <v>50</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="10">
+        <v>10</v>
+      </c>
+      <c r="D11" s="10">
+        <v>15</v>
+      </c>
+      <c r="E11" s="10">
+        <v>20</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10">
+        <v>-5</v>
+      </c>
+      <c r="D12" s="10">
+        <v>-10</v>
+      </c>
+      <c r="E12" s="10">
+        <v>-20</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>